<commit_message>
Add Idare and Kurum models, update Birim structure
Introduced new Idare and Kurum models and updated the Birim model to include an IdareAdi field. Modified templates and views to support selection and display of Idare and Kurum, enhanced reporting and export features to filter by Idare, and improved the print modal for multi-birim selection. Also updated migration files and adjusted related forms, context, and JavaScript logic accordingly.
</commit_message>
<xml_diff>
--- a/PersonelYonSis/staticfiles/excels/HizmetSunumSablon.xlsx
+++ b/PersonelYonSis/staticfiles/excels/HizmetSunumSablon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idare10\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PerYonSis\PersonelYonSis\staticfiles\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>T.C. Kimlik No</t>
   </si>
@@ -46,12 +46,18 @@
   </si>
   <si>
     <t>Sertifika</t>
+  </si>
+  <si>
+    <t>Kurum</t>
+  </si>
+  <si>
+    <t>Üst Birim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -882,9 +888,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -895,9 +903,11 @@
     <col min="6" max="6" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -924,6 +934,12 @@
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>